<commit_message>
Removed 'not used' element cardinality constraints in Claim. Minor example content fixes. Cleanup
Removed 'not used' element cardinality constraints in Claim. Minor example content fixes in ClaimResponse (display values in a couple coded elements). Corrected display value error in billing units value set. Some cleanup of narrative content.
</commit_message>
<xml_diff>
--- a/output/carin-rtpbc-request-Claim.xlsx
+++ b/output/carin-rtpbc-request-Claim.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7635" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7634" uniqueCount="882">
   <si>
     <t>Path</t>
   </si>
@@ -980,7 +980,7 @@
     <t>Claim.enterer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference
+    <t xml:space="preserve">Reference(Practitioner|PractitionerRole)
 </t>
   </si>
   <si>
@@ -2327,10 +2327,7 @@
     <t>Claim.item.serviced[x]</t>
   </si>
   <si>
-    <t>Predetermination is processed as of the request date</t>
-  </si>
-  <si>
-    <t>Predetermination as of request date</t>
+    <t>Date or dates of service or product delivery</t>
   </si>
   <si>
     <t>The date or dates when the service or product was supplied, performed or completed.</t>
@@ -2899,7 +2896,7 @@
     <col min="1" max="1" width="45.46875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="47.5078125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="48.4765625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="33.828125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
@@ -6433,7 +6430,7 @@
         <v>40</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>42</v>
@@ -7413,7 +7410,7 @@
         <v>40</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>42</v>
@@ -7635,7 +7632,7 @@
         <v>40</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>42</v>
@@ -9911,7 +9908,7 @@
         <v>40</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>42</v>
@@ -10021,7 +10018,7 @@
         <v>40</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>42</v>
@@ -10891,7 +10888,7 @@
         <v>40</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>42</v>
@@ -11001,7 +10998,7 @@
         <v>40</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>42</v>
@@ -11653,7 +11650,7 @@
         <v>40</v>
       </c>
       <c r="F81" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G81" t="s" s="2">
         <v>42</v>
@@ -11763,7 +11760,7 @@
         <v>40</v>
       </c>
       <c r="F82" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G82" t="s" s="2">
         <v>42</v>
@@ -13499,7 +13496,7 @@
         <v>40</v>
       </c>
       <c r="F98" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G98" t="s" s="2">
         <v>42</v>
@@ -14585,7 +14582,7 @@
         <v>40</v>
       </c>
       <c r="F108" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G108" t="s" s="2">
         <v>42</v>
@@ -15563,7 +15560,7 @@
         <v>40</v>
       </c>
       <c r="F117" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G117" t="s" s="2">
         <v>42</v>
@@ -18389,7 +18386,7 @@
         <v>40</v>
       </c>
       <c r="F143" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G143" t="s" s="2">
         <v>42</v>
@@ -20127,7 +20124,7 @@
         <v>40</v>
       </c>
       <c r="F159" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G159" t="s" s="2">
         <v>42</v>
@@ -20235,7 +20232,7 @@
         <v>40</v>
       </c>
       <c r="F160" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G160" t="s" s="2">
         <v>42</v>
@@ -21651,7 +21648,7 @@
         <v>40</v>
       </c>
       <c r="F173" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G173" t="s" s="2">
         <v>42</v>
@@ -21761,7 +21758,7 @@
         <v>40</v>
       </c>
       <c r="F174" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G174" t="s" s="2">
         <v>42</v>
@@ -21866,14 +21863,12 @@
       <c r="C175" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="D175" t="s" s="2">
-        <v>747</v>
-      </c>
+      <c r="D175" s="2"/>
       <c r="E175" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F175" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G175" t="s" s="2">
         <v>42</v>
@@ -21888,14 +21883,14 @@
         <v>506</v>
       </c>
       <c r="K175" t="s" s="2">
+        <v>747</v>
+      </c>
+      <c r="L175" t="s" s="2">
         <v>748</v>
-      </c>
-      <c r="L175" t="s" s="2">
-        <v>749</v>
       </c>
       <c r="M175" s="2"/>
       <c r="N175" t="s" s="2">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O175" t="s" s="2">
         <v>42</v>
@@ -21970,7 +21965,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
@@ -21981,7 +21976,7 @@
         <v>40</v>
       </c>
       <c r="F176" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G176" t="s" s="2">
         <v>42</v>
@@ -21993,17 +21988,17 @@
         <v>42</v>
       </c>
       <c r="J176" t="s" s="2">
+        <v>751</v>
+      </c>
+      <c r="K176" t="s" s="2">
         <v>752</v>
       </c>
-      <c r="K176" t="s" s="2">
+      <c r="L176" t="s" s="2">
         <v>753</v>
-      </c>
-      <c r="L176" t="s" s="2">
-        <v>754</v>
       </c>
       <c r="M176" s="2"/>
       <c r="N176" t="s" s="2">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="O176" t="s" s="2">
         <v>42</v>
@@ -22031,11 +22026,11 @@
         <v>250</v>
       </c>
       <c r="X176" t="s" s="2">
+        <v>755</v>
+      </c>
+      <c r="Y176" t="s" s="2">
         <v>756</v>
       </c>
-      <c r="Y176" t="s" s="2">
-        <v>757</v>
-      </c>
       <c r="Z176" t="s" s="2">
         <v>42</v>
       </c>
@@ -22052,7 +22047,7 @@
         <v>42</v>
       </c>
       <c r="AE176" t="s" s="2">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="AF176" t="s" s="2">
         <v>40</v>
@@ -22078,14 +22073,14 @@
     </row>
     <row r="177">
       <c r="A177" t="s" s="2">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D177" t="s" s="2">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E177" t="s" s="2">
         <v>51</v>
@@ -22103,17 +22098,17 @@
         <v>42</v>
       </c>
       <c r="J177" t="s" s="2">
+        <v>759</v>
+      </c>
+      <c r="K177" t="s" s="2">
+        <v>758</v>
+      </c>
+      <c r="L177" t="s" s="2">
         <v>760</v>
-      </c>
-      <c r="K177" t="s" s="2">
-        <v>759</v>
-      </c>
-      <c r="L177" t="s" s="2">
-        <v>761</v>
       </c>
       <c r="M177" s="2"/>
       <c r="N177" t="s" s="2">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="O177" t="s" s="2">
         <v>42</v>
@@ -22162,7 +22157,7 @@
         <v>42</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>40</v>
@@ -22188,7 +22183,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22294,7 +22289,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22402,14 +22397,14 @@
     </row>
     <row r="180">
       <c r="A180" t="s" s="2">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D180" t="s" s="2">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E180" t="s" s="2">
         <v>51</v>
@@ -22427,19 +22422,19 @@
         <v>52</v>
       </c>
       <c r="J180" t="s" s="2">
+        <v>766</v>
+      </c>
+      <c r="K180" t="s" s="2">
+        <v>765</v>
+      </c>
+      <c r="L180" t="s" s="2">
         <v>767</v>
       </c>
-      <c r="K180" t="s" s="2">
-        <v>766</v>
-      </c>
-      <c r="L180" t="s" s="2">
+      <c r="M180" t="s" s="2">
         <v>768</v>
       </c>
-      <c r="M180" t="s" s="2">
+      <c r="N180" t="s" s="2">
         <v>769</v>
-      </c>
-      <c r="N180" t="s" s="2">
-        <v>770</v>
       </c>
       <c r="O180" t="s" s="2">
         <v>42</v>
@@ -22488,7 +22483,7 @@
         <v>42</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>40</v>
@@ -22509,12 +22504,12 @@
         <v>42</v>
       </c>
       <c r="AL180" t="s" s="2">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22540,20 +22535,20 @@
         <v>70</v>
       </c>
       <c r="K181" t="s" s="2">
+        <v>773</v>
+      </c>
+      <c r="L181" t="s" s="2">
         <v>774</v>
-      </c>
-      <c r="L181" t="s" s="2">
-        <v>775</v>
       </c>
       <c r="M181" s="2"/>
       <c r="N181" t="s" s="2">
+        <v>775</v>
+      </c>
+      <c r="O181" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="P181" t="s" s="2">
         <v>776</v>
-      </c>
-      <c r="O181" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="P181" t="s" s="2">
-        <v>777</v>
       </c>
       <c r="Q181" t="s" s="2">
         <v>42</v>
@@ -22577,28 +22572,28 @@
         <v>131</v>
       </c>
       <c r="X181" t="s" s="2">
+        <v>777</v>
+      </c>
+      <c r="Y181" t="s" s="2">
         <v>778</v>
       </c>
-      <c r="Y181" t="s" s="2">
+      <c r="Z181" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA181" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB181" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC181" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD181" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE181" t="s" s="2">
         <v>779</v>
-      </c>
-      <c r="Z181" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA181" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB181" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC181" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD181" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE181" t="s" s="2">
-        <v>780</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>40</v>
@@ -22619,19 +22614,19 @@
         <v>42</v>
       </c>
       <c r="AL181" t="s" s="2">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="s" s="2">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
         <v>42</v>
       </c>
       <c r="D182" t="s" s="2">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E182" t="s" s="2">
         <v>51</v>
@@ -22652,14 +22647,14 @@
         <v>53</v>
       </c>
       <c r="K182" t="s" s="2">
+        <v>782</v>
+      </c>
+      <c r="L182" t="s" s="2">
         <v>783</v>
-      </c>
-      <c r="L182" t="s" s="2">
-        <v>784</v>
       </c>
       <c r="M182" s="2"/>
       <c r="N182" t="s" s="2">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="O182" t="s" s="2">
         <v>42</v>
@@ -22687,28 +22682,28 @@
         <v>131</v>
       </c>
       <c r="X182" t="s" s="2">
+        <v>785</v>
+      </c>
+      <c r="Y182" t="s" s="2">
         <v>786</v>
       </c>
-      <c r="Y182" t="s" s="2">
+      <c r="Z182" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AA182" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AB182" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AC182" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AD182" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AE182" t="s" s="2">
         <v>787</v>
-      </c>
-      <c r="Z182" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AA182" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AB182" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AC182" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AD182" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AE182" t="s" s="2">
-        <v>788</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>40</v>
@@ -22729,12 +22724,12 @@
         <v>42</v>
       </c>
       <c r="AL182" t="s" s="2">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -22760,14 +22755,14 @@
         <v>64</v>
       </c>
       <c r="K183" t="s" s="2">
+        <v>790</v>
+      </c>
+      <c r="L183" t="s" s="2">
         <v>791</v>
-      </c>
-      <c r="L183" t="s" s="2">
-        <v>792</v>
       </c>
       <c r="M183" s="2"/>
       <c r="N183" t="s" s="2">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="O183" t="s" s="2">
         <v>42</v>
@@ -22816,16 +22811,16 @@
         <v>42</v>
       </c>
       <c r="AE183" t="s" s="2">
+        <v>793</v>
+      </c>
+      <c r="AF183" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG183" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="AH183" t="s" s="2">
         <v>794</v>
-      </c>
-      <c r="AF183" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG183" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH183" t="s" s="2">
-        <v>795</v>
       </c>
       <c r="AI183" t="s" s="2">
         <v>62</v>
@@ -22837,12 +22832,12 @@
         <v>42</v>
       </c>
       <c r="AL183" t="s" s="2">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="184" hidden="true">
       <c r="A184" t="s" s="2">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -22868,16 +22863,16 @@
         <v>70</v>
       </c>
       <c r="K184" t="s" s="2">
+        <v>797</v>
+      </c>
+      <c r="L184" t="s" s="2">
         <v>798</v>
       </c>
-      <c r="L184" t="s" s="2">
+      <c r="M184" t="s" s="2">
         <v>799</v>
       </c>
-      <c r="M184" t="s" s="2">
+      <c r="N184" t="s" s="2">
         <v>800</v>
-      </c>
-      <c r="N184" t="s" s="2">
-        <v>801</v>
       </c>
       <c r="O184" t="s" s="2">
         <v>42</v>
@@ -22926,7 +22921,7 @@
         <v>42</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>40</v>
@@ -22947,12 +22942,12 @@
         <v>42</v>
       </c>
       <c r="AL184" t="s" s="2">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -22963,7 +22958,7 @@
         <v>40</v>
       </c>
       <c r="F185" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G185" t="s" s="2">
         <v>42</v>
@@ -22975,17 +22970,17 @@
         <v>42</v>
       </c>
       <c r="J185" t="s" s="2">
+        <v>804</v>
+      </c>
+      <c r="K185" t="s" s="2">
         <v>805</v>
       </c>
-      <c r="K185" t="s" s="2">
+      <c r="L185" t="s" s="2">
         <v>806</v>
-      </c>
-      <c r="L185" t="s" s="2">
-        <v>807</v>
       </c>
       <c r="M185" s="2"/>
       <c r="N185" t="s" s="2">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="O185" t="s" s="2">
         <v>42</v>
@@ -23034,7 +23029,7 @@
         <v>42</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>40</v>
@@ -23060,7 +23055,7 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
@@ -23071,7 +23066,7 @@
         <v>40</v>
       </c>
       <c r="F186" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G186" t="s" s="2">
         <v>42</v>
@@ -23083,19 +23078,19 @@
         <v>42</v>
       </c>
       <c r="J186" t="s" s="2">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="K186" t="s" s="2">
+        <v>809</v>
+      </c>
+      <c r="L186" t="s" s="2">
         <v>810</v>
       </c>
-      <c r="L186" t="s" s="2">
+      <c r="M186" t="s" s="2">
         <v>811</v>
       </c>
-      <c r="M186" t="s" s="2">
+      <c r="N186" t="s" s="2">
         <v>812</v>
-      </c>
-      <c r="N186" t="s" s="2">
-        <v>813</v>
       </c>
       <c r="O186" t="s" s="2">
         <v>42</v>
@@ -23144,7 +23139,7 @@
         <v>42</v>
       </c>
       <c r="AE186" t="s" s="2">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="AF186" t="s" s="2">
         <v>40</v>
@@ -23170,7 +23165,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -23181,7 +23176,7 @@
         <v>40</v>
       </c>
       <c r="F187" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G187" t="s" s="2">
         <v>42</v>
@@ -23193,19 +23188,19 @@
         <v>42</v>
       </c>
       <c r="J187" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K187" t="s" s="2">
+        <v>814</v>
+      </c>
+      <c r="L187" t="s" s="2">
         <v>815</v>
       </c>
-      <c r="L187" t="s" s="2">
+      <c r="M187" t="s" s="2">
         <v>816</v>
       </c>
-      <c r="M187" t="s" s="2">
+      <c r="N187" t="s" s="2">
         <v>817</v>
-      </c>
-      <c r="N187" t="s" s="2">
-        <v>818</v>
       </c>
       <c r="O187" t="s" s="2">
         <v>42</v>
@@ -23254,7 +23249,7 @@
         <v>42</v>
       </c>
       <c r="AE187" t="s" s="2">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="AF187" t="s" s="2">
         <v>40</v>
@@ -23280,7 +23275,7 @@
     </row>
     <row r="188" hidden="true">
       <c r="A188" t="s" s="2">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B188" s="2"/>
       <c r="C188" t="s" s="2">
@@ -23362,7 +23357,7 @@
         <v>42</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>40</v>
@@ -23388,7 +23383,7 @@
     </row>
     <row r="189" hidden="true">
       <c r="A189" t="s" s="2">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
@@ -23399,7 +23394,7 @@
         <v>40</v>
       </c>
       <c r="F189" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G189" t="s" s="2">
         <v>42</v>
@@ -23414,16 +23409,16 @@
         <v>137</v>
       </c>
       <c r="K189" t="s" s="2">
+        <v>820</v>
+      </c>
+      <c r="L189" t="s" s="2">
         <v>821</v>
       </c>
-      <c r="L189" t="s" s="2">
+      <c r="M189" t="s" s="2">
         <v>822</v>
       </c>
-      <c r="M189" t="s" s="2">
+      <c r="N189" t="s" s="2">
         <v>823</v>
-      </c>
-      <c r="N189" t="s" s="2">
-        <v>824</v>
       </c>
       <c r="O189" t="s" s="2">
         <v>42</v>
@@ -23451,11 +23446,11 @@
         <v>250</v>
       </c>
       <c r="X189" t="s" s="2">
+        <v>824</v>
+      </c>
+      <c r="Y189" t="s" s="2">
         <v>825</v>
       </c>
-      <c r="Y189" t="s" s="2">
-        <v>826</v>
-      </c>
       <c r="Z189" t="s" s="2">
         <v>42</v>
       </c>
@@ -23472,7 +23467,7 @@
         <v>42</v>
       </c>
       <c r="AE189" t="s" s="2">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="AF189" t="s" s="2">
         <v>40</v>
@@ -23498,7 +23493,7 @@
     </row>
     <row r="190" hidden="true">
       <c r="A190" t="s" s="2">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B190" s="2"/>
       <c r="C190" t="s" s="2">
@@ -23509,7 +23504,7 @@
         <v>40</v>
       </c>
       <c r="F190" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G190" t="s" s="2">
         <v>42</v>
@@ -23524,14 +23519,14 @@
         <v>137</v>
       </c>
       <c r="K190" t="s" s="2">
+        <v>827</v>
+      </c>
+      <c r="L190" t="s" s="2">
         <v>828</v>
-      </c>
-      <c r="L190" t="s" s="2">
-        <v>829</v>
       </c>
       <c r="M190" s="2"/>
       <c r="N190" t="s" s="2">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="O190" t="s" s="2">
         <v>42</v>
@@ -23559,11 +23554,11 @@
         <v>250</v>
       </c>
       <c r="X190" t="s" s="2">
+        <v>829</v>
+      </c>
+      <c r="Y190" t="s" s="2">
         <v>830</v>
       </c>
-      <c r="Y190" t="s" s="2">
-        <v>831</v>
-      </c>
       <c r="Z190" t="s" s="2">
         <v>42</v>
       </c>
@@ -23580,7 +23575,7 @@
         <v>42</v>
       </c>
       <c r="AE190" t="s" s="2">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="AF190" t="s" s="2">
         <v>40</v>
@@ -23606,7 +23601,7 @@
     </row>
     <row r="191" hidden="true">
       <c r="A191" t="s" s="2">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" t="s" s="2">
@@ -23617,7 +23612,7 @@
         <v>40</v>
       </c>
       <c r="F191" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G191" t="s" s="2">
         <v>42</v>
@@ -23629,19 +23624,19 @@
         <v>42</v>
       </c>
       <c r="J191" t="s" s="2">
+        <v>832</v>
+      </c>
+      <c r="K191" t="s" s="2">
         <v>833</v>
       </c>
-      <c r="K191" t="s" s="2">
+      <c r="L191" t="s" s="2">
         <v>834</v>
       </c>
-      <c r="L191" t="s" s="2">
+      <c r="M191" t="s" s="2">
         <v>835</v>
       </c>
-      <c r="M191" t="s" s="2">
+      <c r="N191" t="s" s="2">
         <v>836</v>
-      </c>
-      <c r="N191" t="s" s="2">
-        <v>837</v>
       </c>
       <c r="O191" t="s" s="2">
         <v>42</v>
@@ -23690,7 +23685,7 @@
         <v>42</v>
       </c>
       <c r="AE191" t="s" s="2">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="AF191" t="s" s="2">
         <v>40</v>
@@ -23705,7 +23700,7 @@
         <v>62</v>
       </c>
       <c r="AJ191" t="s" s="2">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="AK191" t="s" s="2">
         <v>42</v>
@@ -23716,7 +23711,7 @@
     </row>
     <row r="192" hidden="true">
       <c r="A192" t="s" s="2">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
@@ -23727,7 +23722,7 @@
         <v>40</v>
       </c>
       <c r="F192" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G192" t="s" s="2">
         <v>42</v>
@@ -23742,10 +23737,10 @@
         <v>362</v>
       </c>
       <c r="K192" t="s" s="2">
+        <v>839</v>
+      </c>
+      <c r="L192" t="s" s="2">
         <v>840</v>
-      </c>
-      <c r="L192" t="s" s="2">
-        <v>841</v>
       </c>
       <c r="M192" s="2"/>
       <c r="N192" t="s" s="2">
@@ -23798,7 +23793,7 @@
         <v>42</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>40</v>
@@ -23824,7 +23819,7 @@
     </row>
     <row r="193" hidden="true">
       <c r="A193" t="s" s="2">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B193" s="2"/>
       <c r="C193" t="s" s="2">
@@ -23930,7 +23925,7 @@
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -24038,7 +24033,7 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
@@ -24148,7 +24143,7 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -24230,7 +24225,7 @@
         <v>42</v>
       </c>
       <c r="AE196" t="s" s="2">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="AF196" t="s" s="2">
         <v>51</v>
@@ -24256,7 +24251,7 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -24338,7 +24333,7 @@
         <v>42</v>
       </c>
       <c r="AE197" t="s" s="2">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="AF197" t="s" s="2">
         <v>40</v>
@@ -24364,7 +24359,7 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
@@ -24448,7 +24443,7 @@
         <v>42</v>
       </c>
       <c r="AE198" t="s" s="2">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="AF198" t="s" s="2">
         <v>40</v>
@@ -24474,7 +24469,7 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
@@ -24500,13 +24495,13 @@
         <v>137</v>
       </c>
       <c r="K199" t="s" s="2">
+        <v>848</v>
+      </c>
+      <c r="L199" t="s" s="2">
         <v>849</v>
       </c>
-      <c r="L199" t="s" s="2">
+      <c r="M199" t="s" s="2">
         <v>850</v>
-      </c>
-      <c r="M199" t="s" s="2">
-        <v>851</v>
       </c>
       <c r="N199" t="s" s="2">
         <v>716</v>
@@ -24537,11 +24532,11 @@
         <v>250</v>
       </c>
       <c r="X199" t="s" s="2">
+        <v>851</v>
+      </c>
+      <c r="Y199" t="s" s="2">
         <v>852</v>
       </c>
-      <c r="Y199" t="s" s="2">
-        <v>853</v>
-      </c>
       <c r="Z199" t="s" s="2">
         <v>42</v>
       </c>
@@ -24558,7 +24553,7 @@
         <v>42</v>
       </c>
       <c r="AE199" t="s" s="2">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="AF199" t="s" s="2">
         <v>51</v>
@@ -24584,7 +24579,7 @@
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -24610,13 +24605,13 @@
         <v>137</v>
       </c>
       <c r="K200" t="s" s="2">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="L200" t="s" s="2">
         <v>734</v>
       </c>
       <c r="M200" t="s" s="2">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="N200" t="s" s="2">
         <v>736</v>
@@ -24668,7 +24663,7 @@
         <v>42</v>
       </c>
       <c r="AE200" t="s" s="2">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="AF200" t="s" s="2">
         <v>40</v>
@@ -24694,7 +24689,7 @@
     </row>
     <row r="201" hidden="true">
       <c r="A201" t="s" s="2">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B201" s="2"/>
       <c r="C201" t="s" s="2">
@@ -24778,7 +24773,7 @@
         <v>42</v>
       </c>
       <c r="AE201" t="s" s="2">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="AF201" t="s" s="2">
         <v>40</v>
@@ -24804,7 +24799,7 @@
     </row>
     <row r="202" hidden="true">
       <c r="A202" t="s" s="2">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B202" s="2"/>
       <c r="C202" t="s" s="2">
@@ -24827,17 +24822,17 @@
         <v>42</v>
       </c>
       <c r="J202" t="s" s="2">
+        <v>759</v>
+      </c>
+      <c r="K202" t="s" s="2">
+        <v>858</v>
+      </c>
+      <c r="L202" t="s" s="2">
         <v>760</v>
-      </c>
-      <c r="K202" t="s" s="2">
-        <v>859</v>
-      </c>
-      <c r="L202" t="s" s="2">
-        <v>761</v>
       </c>
       <c r="M202" s="2"/>
       <c r="N202" t="s" s="2">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="O202" t="s" s="2">
         <v>42</v>
@@ -24886,7 +24881,7 @@
         <v>42</v>
       </c>
       <c r="AE202" t="s" s="2">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="AF202" t="s" s="2">
         <v>40</v>
@@ -24912,7 +24907,7 @@
     </row>
     <row r="203" hidden="true">
       <c r="A203" t="s" s="2">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B203" s="2"/>
       <c r="C203" t="s" s="2">
@@ -24935,17 +24930,17 @@
         <v>42</v>
       </c>
       <c r="J203" t="s" s="2">
+        <v>804</v>
+      </c>
+      <c r="K203" t="s" s="2">
         <v>805</v>
       </c>
-      <c r="K203" t="s" s="2">
+      <c r="L203" t="s" s="2">
         <v>806</v>
-      </c>
-      <c r="L203" t="s" s="2">
-        <v>807</v>
       </c>
       <c r="M203" s="2"/>
       <c r="N203" t="s" s="2">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="O203" t="s" s="2">
         <v>42</v>
@@ -24994,7 +24989,7 @@
         <v>42</v>
       </c>
       <c r="AE203" t="s" s="2">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="AF203" t="s" s="2">
         <v>40</v>
@@ -25020,7 +25015,7 @@
     </row>
     <row r="204" hidden="true">
       <c r="A204" t="s" s="2">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B204" s="2"/>
       <c r="C204" t="s" s="2">
@@ -25043,19 +25038,19 @@
         <v>42</v>
       </c>
       <c r="J204" t="s" s="2">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="K204" t="s" s="2">
+        <v>809</v>
+      </c>
+      <c r="L204" t="s" s="2">
         <v>810</v>
       </c>
-      <c r="L204" t="s" s="2">
+      <c r="M204" t="s" s="2">
         <v>811</v>
       </c>
-      <c r="M204" t="s" s="2">
+      <c r="N204" t="s" s="2">
         <v>812</v>
-      </c>
-      <c r="N204" t="s" s="2">
-        <v>813</v>
       </c>
       <c r="O204" t="s" s="2">
         <v>42</v>
@@ -25104,7 +25099,7 @@
         <v>42</v>
       </c>
       <c r="AE204" t="s" s="2">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="AF204" t="s" s="2">
         <v>40</v>
@@ -25130,7 +25125,7 @@
     </row>
     <row r="205" hidden="true">
       <c r="A205" t="s" s="2">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B205" s="2"/>
       <c r="C205" t="s" s="2">
@@ -25153,19 +25148,19 @@
         <v>42</v>
       </c>
       <c r="J205" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K205" t="s" s="2">
+        <v>814</v>
+      </c>
+      <c r="L205" t="s" s="2">
         <v>815</v>
       </c>
-      <c r="L205" t="s" s="2">
+      <c r="M205" t="s" s="2">
         <v>816</v>
       </c>
-      <c r="M205" t="s" s="2">
+      <c r="N205" t="s" s="2">
         <v>817</v>
-      </c>
-      <c r="N205" t="s" s="2">
-        <v>818</v>
       </c>
       <c r="O205" t="s" s="2">
         <v>42</v>
@@ -25214,7 +25209,7 @@
         <v>42</v>
       </c>
       <c r="AE205" t="s" s="2">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="AF205" t="s" s="2">
         <v>40</v>
@@ -25240,7 +25235,7 @@
     </row>
     <row r="206" hidden="true">
       <c r="A206" t="s" s="2">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" t="s" s="2">
@@ -25322,7 +25317,7 @@
         <v>42</v>
       </c>
       <c r="AE206" t="s" s="2">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="AF206" t="s" s="2">
         <v>40</v>
@@ -25348,7 +25343,7 @@
     </row>
     <row r="207" hidden="true">
       <c r="A207" t="s" s="2">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B207" s="2"/>
       <c r="C207" t="s" s="2">
@@ -25374,10 +25369,10 @@
         <v>362</v>
       </c>
       <c r="K207" t="s" s="2">
+        <v>839</v>
+      </c>
+      <c r="L207" t="s" s="2">
         <v>840</v>
-      </c>
-      <c r="L207" t="s" s="2">
-        <v>841</v>
       </c>
       <c r="M207" s="2"/>
       <c r="N207" t="s" s="2">
@@ -25430,7 +25425,7 @@
         <v>42</v>
       </c>
       <c r="AE207" t="s" s="2">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="AF207" t="s" s="2">
         <v>40</v>
@@ -25456,7 +25451,7 @@
     </row>
     <row r="208" hidden="true">
       <c r="A208" t="s" s="2">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B208" s="2"/>
       <c r="C208" t="s" s="2">
@@ -25562,7 +25557,7 @@
     </row>
     <row r="209" hidden="true">
       <c r="A209" t="s" s="2">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B209" s="2"/>
       <c r="C209" t="s" s="2">
@@ -25670,7 +25665,7 @@
     </row>
     <row r="210" hidden="true">
       <c r="A210" t="s" s="2">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" t="s" s="2">
@@ -25780,7 +25775,7 @@
     </row>
     <row r="211" hidden="true">
       <c r="A211" t="s" s="2">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B211" s="2"/>
       <c r="C211" t="s" s="2">
@@ -25862,7 +25857,7 @@
         <v>42</v>
       </c>
       <c r="AE211" t="s" s="2">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="AF211" t="s" s="2">
         <v>51</v>
@@ -25888,7 +25883,7 @@
     </row>
     <row r="212" hidden="true">
       <c r="A212" t="s" s="2">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" t="s" s="2">
@@ -25970,7 +25965,7 @@
         <v>42</v>
       </c>
       <c r="AE212" t="s" s="2">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="AF212" t="s" s="2">
         <v>40</v>
@@ -25996,7 +25991,7 @@
     </row>
     <row r="213" hidden="true">
       <c r="A213" t="s" s="2">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B213" s="2"/>
       <c r="C213" t="s" s="2">
@@ -26080,7 +26075,7 @@
         <v>42</v>
       </c>
       <c r="AE213" t="s" s="2">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="AF213" t="s" s="2">
         <v>40</v>
@@ -26106,7 +26101,7 @@
     </row>
     <row r="214" hidden="true">
       <c r="A214" t="s" s="2">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B214" s="2"/>
       <c r="C214" t="s" s="2">
@@ -26132,13 +26127,13 @@
         <v>137</v>
       </c>
       <c r="K214" t="s" s="2">
+        <v>848</v>
+      </c>
+      <c r="L214" t="s" s="2">
         <v>849</v>
       </c>
-      <c r="L214" t="s" s="2">
+      <c r="M214" t="s" s="2">
         <v>850</v>
-      </c>
-      <c r="M214" t="s" s="2">
-        <v>851</v>
       </c>
       <c r="N214" t="s" s="2">
         <v>716</v>
@@ -26169,11 +26164,11 @@
         <v>250</v>
       </c>
       <c r="X214" t="s" s="2">
+        <v>851</v>
+      </c>
+      <c r="Y214" t="s" s="2">
         <v>852</v>
       </c>
-      <c r="Y214" t="s" s="2">
-        <v>853</v>
-      </c>
       <c r="Z214" t="s" s="2">
         <v>42</v>
       </c>
@@ -26190,7 +26185,7 @@
         <v>42</v>
       </c>
       <c r="AE214" t="s" s="2">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="AF214" t="s" s="2">
         <v>51</v>
@@ -26216,7 +26211,7 @@
     </row>
     <row r="215" hidden="true">
       <c r="A215" t="s" s="2">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B215" s="2"/>
       <c r="C215" t="s" s="2">
@@ -26242,13 +26237,13 @@
         <v>137</v>
       </c>
       <c r="K215" t="s" s="2">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="L215" t="s" s="2">
         <v>734</v>
       </c>
       <c r="M215" t="s" s="2">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="N215" t="s" s="2">
         <v>736</v>
@@ -26300,7 +26295,7 @@
         <v>42</v>
       </c>
       <c r="AE215" t="s" s="2">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="AF215" t="s" s="2">
         <v>40</v>
@@ -26326,7 +26321,7 @@
     </row>
     <row r="216" hidden="true">
       <c r="A216" t="s" s="2">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B216" s="2"/>
       <c r="C216" t="s" s="2">
@@ -26410,7 +26405,7 @@
         <v>42</v>
       </c>
       <c r="AE216" t="s" s="2">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="AF216" t="s" s="2">
         <v>40</v>
@@ -26436,7 +26431,7 @@
     </row>
     <row r="217" hidden="true">
       <c r="A217" t="s" s="2">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B217" s="2"/>
       <c r="C217" t="s" s="2">
@@ -26459,17 +26454,17 @@
         <v>42</v>
       </c>
       <c r="J217" t="s" s="2">
+        <v>759</v>
+      </c>
+      <c r="K217" t="s" s="2">
+        <v>858</v>
+      </c>
+      <c r="L217" t="s" s="2">
         <v>760</v>
-      </c>
-      <c r="K217" t="s" s="2">
-        <v>859</v>
-      </c>
-      <c r="L217" t="s" s="2">
-        <v>761</v>
       </c>
       <c r="M217" s="2"/>
       <c r="N217" t="s" s="2">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="O217" t="s" s="2">
         <v>42</v>
@@ -26518,7 +26513,7 @@
         <v>42</v>
       </c>
       <c r="AE217" t="s" s="2">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="AF217" t="s" s="2">
         <v>40</v>
@@ -26544,7 +26539,7 @@
     </row>
     <row r="218" hidden="true">
       <c r="A218" t="s" s="2">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B218" s="2"/>
       <c r="C218" t="s" s="2">
@@ -26567,17 +26562,17 @@
         <v>42</v>
       </c>
       <c r="J218" t="s" s="2">
+        <v>804</v>
+      </c>
+      <c r="K218" t="s" s="2">
         <v>805</v>
       </c>
-      <c r="K218" t="s" s="2">
+      <c r="L218" t="s" s="2">
         <v>806</v>
-      </c>
-      <c r="L218" t="s" s="2">
-        <v>807</v>
       </c>
       <c r="M218" s="2"/>
       <c r="N218" t="s" s="2">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="O218" t="s" s="2">
         <v>42</v>
@@ -26626,7 +26621,7 @@
         <v>42</v>
       </c>
       <c r="AE218" t="s" s="2">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="AF218" t="s" s="2">
         <v>40</v>
@@ -26652,7 +26647,7 @@
     </row>
     <row r="219" hidden="true">
       <c r="A219" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B219" s="2"/>
       <c r="C219" t="s" s="2">
@@ -26675,19 +26670,19 @@
         <v>42</v>
       </c>
       <c r="J219" t="s" s="2">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="K219" t="s" s="2">
+        <v>809</v>
+      </c>
+      <c r="L219" t="s" s="2">
         <v>810</v>
       </c>
-      <c r="L219" t="s" s="2">
+      <c r="M219" t="s" s="2">
         <v>811</v>
       </c>
-      <c r="M219" t="s" s="2">
+      <c r="N219" t="s" s="2">
         <v>812</v>
-      </c>
-      <c r="N219" t="s" s="2">
-        <v>813</v>
       </c>
       <c r="O219" t="s" s="2">
         <v>42</v>
@@ -26736,7 +26731,7 @@
         <v>42</v>
       </c>
       <c r="AE219" t="s" s="2">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="AF219" t="s" s="2">
         <v>40</v>
@@ -26762,7 +26757,7 @@
     </row>
     <row r="220" hidden="true">
       <c r="A220" t="s" s="2">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B220" s="2"/>
       <c r="C220" t="s" s="2">
@@ -26785,19 +26780,19 @@
         <v>42</v>
       </c>
       <c r="J220" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K220" t="s" s="2">
+        <v>814</v>
+      </c>
+      <c r="L220" t="s" s="2">
         <v>815</v>
       </c>
-      <c r="L220" t="s" s="2">
+      <c r="M220" t="s" s="2">
         <v>816</v>
       </c>
-      <c r="M220" t="s" s="2">
+      <c r="N220" t="s" s="2">
         <v>817</v>
-      </c>
-      <c r="N220" t="s" s="2">
-        <v>818</v>
       </c>
       <c r="O220" t="s" s="2">
         <v>42</v>
@@ -26846,7 +26841,7 @@
         <v>42</v>
       </c>
       <c r="AE220" t="s" s="2">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="AF220" t="s" s="2">
         <v>40</v>
@@ -26872,7 +26867,7 @@
     </row>
     <row r="221" hidden="true">
       <c r="A221" t="s" s="2">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B221" s="2"/>
       <c r="C221" t="s" s="2">
@@ -26954,7 +26949,7 @@
         <v>42</v>
       </c>
       <c r="AE221" t="s" s="2">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="AF221" t="s" s="2">
         <v>40</v>
@@ -26980,7 +26975,7 @@
     </row>
     <row r="222" hidden="true">
       <c r="A222" t="s" s="2">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B222" s="2"/>
       <c r="C222" t="s" s="2">
@@ -26991,7 +26986,7 @@
         <v>40</v>
       </c>
       <c r="F222" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G222" t="s" s="2">
         <v>42</v>
@@ -27003,17 +26998,17 @@
         <v>42</v>
       </c>
       <c r="J222" t="s" s="2">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="K222" t="s" s="2">
+        <v>879</v>
+      </c>
+      <c r="L222" t="s" s="2">
         <v>880</v>
-      </c>
-      <c r="L222" t="s" s="2">
-        <v>881</v>
       </c>
       <c r="M222" s="2"/>
       <c r="N222" t="s" s="2">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="O222" t="s" s="2">
         <v>42</v>
@@ -27062,7 +27057,7 @@
         <v>42</v>
       </c>
       <c r="AE222" t="s" s="2">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="AF222" t="s" s="2">
         <v>40</v>

</xml_diff>